<commit_message>
Adding one more test case and Custom Annotation to the framework
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestScript.xlsx
+++ b/src/test/resources/excel/TestScript.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="25">
   <si>
     <t>testname</t>
   </si>
@@ -58,6 +58,39 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>validateUpdateMyInfoTest</t>
+  </si>
+  <si>
+    <t>This test is to validate update feature of My Info</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>Abhishek</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>empid</t>
+  </si>
+  <si>
+    <t>765507</t>
+  </si>
+  <si>
+    <t>dropdownvalue</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -93,8 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,16 +423,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -431,6 +465,17 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -441,10 +486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -452,9 +497,11 @@
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +514,20 @@
       <c r="D1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -481,13 +540,25 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -495,13 +566,25 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -509,13 +592,25 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -523,13 +618,25 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -537,19 +644,69 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementing Encoder -Decoder and webdriverManager to the Framework
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestScript.xlsx
+++ b/src/test/resources/excel/TestScript.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Admin1</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
     <t>validateUpdateMyInfoTest</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM=</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -470,10 +470,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -488,15 +488,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -515,16 +515,16 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -537,20 +537,20 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -563,20 +563,20 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -589,20 +589,20 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -615,20 +615,20 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -641,20 +641,20 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
-        <v>13</v>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -667,25 +667,25 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
-        <v>13</v>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -693,20 +693,20 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>13</v>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>